<commit_message>
making a plot for adjusted and unadjusted for main paper
</commit_message>
<xml_diff>
--- a/tables/table2.xlsx
+++ b/tables/table2.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1828,60 +1828,184 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>Cognitive Difficulty</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Independence Difficulty</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>N</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>79658</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>23021</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>8980</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>21242</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>20064</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>25003</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>352960</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>120724</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>313063</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="K32" t="inlineStr">
         <is>
           <t>3165675</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>94162</t>
         </is>

</xml_diff>